<commit_message>
try to fix databese settings and usege
</commit_message>
<xml_diff>
--- a/Шаблон соревнований.xlsx
+++ b/Шаблон соревнований.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voyte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Projects\Scoreboard_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,9 +49,6 @@
     <t>Пришел</t>
   </si>
   <si>
-    <t>Вес кат</t>
-  </si>
-  <si>
     <t>Группа</t>
   </si>
   <si>
@@ -124,7 +121,10 @@
     <t>Таиров Дамир</t>
   </si>
   <si>
-    <t>Побед</t>
+    <t>Весовая_категория</t>
+  </si>
+  <si>
+    <t>Побед|Встреч</t>
   </si>
 </sst>
 </file>
@@ -509,13 +509,14 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
@@ -534,184 +535,184 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>33288</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>43534</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>38384</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>38444</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
         <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>38902</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>38058</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
         <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add upload data with start app
</commit_message>
<xml_diff>
--- a/Шаблон соревнований.xlsx
+++ b/Шаблон соревнований.xlsx
@@ -35,41 +35,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Спортсмен</t>
   </si>
   <si>
-    <t>Год рождения</t>
-  </si>
-  <si>
-    <t>Оплата</t>
-  </si>
-  <si>
-    <t>Пришел</t>
-  </si>
-  <si>
-    <t>Группа</t>
-  </si>
-  <si>
     <t>Место</t>
   </si>
   <si>
     <t>Команда</t>
   </si>
   <si>
-    <t>Наставник</t>
-  </si>
-  <si>
     <t>Ананьев Матвей Денисович</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Макаров Егор Андреевич</t>
   </si>
   <si>
@@ -79,9 +58,6 @@
     <t xml:space="preserve">Химки 31 школа  </t>
   </si>
   <si>
-    <t xml:space="preserve">Ибрагимов Лёми </t>
-  </si>
-  <si>
     <t>Иванов Иван Иванович</t>
   </si>
   <si>
@@ -106,37 +82,30 @@
     <t>СОШ №582</t>
   </si>
   <si>
-    <t>Антонов Алексей</t>
-  </si>
-  <si>
-    <t>Смелов Егор</t>
-  </si>
-  <si>
-    <t>Шмелев Вячислав</t>
-  </si>
-  <si>
-    <t>Друзь Иван</t>
-  </si>
-  <si>
-    <t>Таиров Дамир</t>
-  </si>
-  <si>
-    <t>Весовая_категория</t>
-  </si>
-  <si>
-    <t>Побед|Встреч</t>
+    <t>Побед|Поражений</t>
+  </si>
+  <si>
+    <t>Весовая</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
@@ -161,16 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,214 +472,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="17.399999999999999">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>33288</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
         <v>22</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43534</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>38384</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>38444</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>38902</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C7" s="1">
         <v>22</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1">
-        <v>38058</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add change to members and teams
</commit_message>
<xml_diff>
--- a/Шаблон соревнований.xlsx
+++ b/Шаблон соревнований.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Projects\Scoreboard_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Projects\Scoreboard_2\Scoreboard_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CAC1BC-AB0E-460B-836B-C6C10F96CF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -91,8 +81,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -471,23 +461,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.296875" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="20.69921875" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="17.399999999999999">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,7 +494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -516,7 +506,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -528,7 +518,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -540,7 +530,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -552,7 +542,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -564,7 +554,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>

</xml_diff>